<commit_message>
Fix dataset: corrected riding_style and codes for bikes
</commit_message>
<xml_diff>
--- a/completed_bike_dataset.xlsx
+++ b/completed_bike_dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Degree 3rd Year\FYP\bikeproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FAC1BB2-051E-4799-A628-B3A8CADFA55E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DD26E9-8EE6-4BC5-ABE6-5FA512DC2065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1113,8 +1113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F321"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F157" sqref="F157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2438,10 +2438,10 @@
         <v>750</v>
       </c>
       <c r="E66" t="s">
-        <v>103</v>
+        <v>46</v>
       </c>
       <c r="F66">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2678,10 +2678,10 @@
         <v>750</v>
       </c>
       <c r="E78" t="s">
-        <v>103</v>
+        <v>46</v>
       </c>
       <c r="F78">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -4038,10 +4038,10 @@
         <v>1000</v>
       </c>
       <c r="E146" t="s">
-        <v>103</v>
+        <v>46</v>
       </c>
       <c r="F146">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
@@ -4258,10 +4258,10 @@
         <v>750</v>
       </c>
       <c r="E157" t="s">
-        <v>103</v>
+        <v>46</v>
       </c>
       <c r="F157">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update dataset: corrected riding_style and codes for accuracy
</commit_message>
<xml_diff>
--- a/completed_bike_dataset.xlsx
+++ b/completed_bike_dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Degree 3rd Year\FYP\bikeproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA07909-8447-4227-939D-0A51AC1A914C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E656E898-3642-4E4A-985A-F2D111C65E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1116,8 +1116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F313"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2361,10 +2361,10 @@
         <v>750</v>
       </c>
       <c r="E62" t="s">
-        <v>8</v>
+        <v>210</v>
       </c>
       <c r="F62">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -3141,10 +3141,10 @@
         <v>650</v>
       </c>
       <c r="E101" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F101">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -3261,10 +3261,10 @@
         <v>650</v>
       </c>
       <c r="E107" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="F107">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -3281,10 +3281,10 @@
         <v>650</v>
       </c>
       <c r="E108" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="F108">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -3401,10 +3401,10 @@
         <v>650</v>
       </c>
       <c r="E114" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="F114">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3761,10 +3761,10 @@
         <v>650</v>
       </c>
       <c r="E132" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="F132">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -3881,10 +3881,10 @@
         <v>650</v>
       </c>
       <c r="E138" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="F138">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>